<commit_message>
fixed equation in ABC_fit.py
</commit_message>
<xml_diff>
--- a/data/VMN_ad_mp_0.8m.xlsx
+++ b/data/VMN_ad_mp_0.8m.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11211"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcofking/Documents/GitHub/ciarrai/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38F489A6-9B64-C44B-8C58-6CF5F1D1C9A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CB5A2E7-750D-294E-9CAC-24E4D7E0733A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25500" yWindow="4020" windowWidth="47620" windowHeight="27680" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -186,6 +186,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -215,11 +218,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="45" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -318,7 +323,7 @@
             <c:numRef>
               <c:f>mass_conc!$A$2:$A$136</c:f>
               <c:numCache>
-                <c:formatCode>mm:ss</c:formatCode>
+                <c:formatCode>[$-F400]h:mm:ss\ am/pm</c:formatCode>
                 <c:ptCount val="135"/>
                 <c:pt idx="0">
                   <c:v>2.3148148148148146E-4</c:v>
@@ -1180,7 +1185,7 @@
             <c:numRef>
               <c:f>mass_conc!$A$2:$A$136</c:f>
               <c:numCache>
-                <c:formatCode>mm:ss</c:formatCode>
+                <c:formatCode>[$-F400]h:mm:ss\ am/pm</c:formatCode>
                 <c:ptCount val="135"/>
                 <c:pt idx="0">
                   <c:v>2.3148148148148146E-4</c:v>
@@ -2043,7 +2048,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="mm:ss" sourceLinked="1"/>
+        <c:numFmt formatCode="[$-F400]h:mm:ss\ am/pm" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2273,494 +2278,418 @@
         <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="2"/>
+          <c:idx val="3"/>
           <c:order val="0"/>
           <c:xVal>
             <c:numRef>
-              <c:f>mass_conc!$A$43:$A$50</c:f>
+              <c:f>mass_conc!$D$2:$D$136</c:f>
               <c:numCache>
-                <c:formatCode>mm:ss</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>9.7222222222222206E-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>9.9537037037037007E-3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.01851851851852E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.0416666666666701E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.06481481481482E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.08796296296296E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.1111111111111099E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.13425925925926E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>mass_conc!$B$43:$B$50</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>8.8846999999999995E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5.61129E-2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.6887399999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.36373E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.2617999999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2.1260899999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2.2346700000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2.0624300000000002E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-9FC6-BB44-B92A-34448F78CDCB}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="1"/>
-          <c:xVal>
-            <c:numRef>
-              <c:f>mass_conc!$A$2:$A$136</c:f>
-              <c:numCache>
-                <c:formatCode>mm:ss</c:formatCode>
+                <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="135"/>
                 <c:pt idx="0">
-                  <c:v>2.3148148148148146E-4</c:v>
+                  <c:v>5.5555555555555549E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.6296296296296293E-4</c:v>
+                  <c:v>1.111111111111111E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.9444444444444447E-4</c:v>
+                  <c:v>1.6666666666666666E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.2592592592592596E-4</c:v>
+                  <c:v>2.2222222222222223E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.1574074074074099E-3</c:v>
+                  <c:v>2.7777777777777839E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.38888888888889E-3</c:v>
+                  <c:v>3.3333333333333361E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.6203703703703701E-3</c:v>
+                  <c:v>3.8888888888888883E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.85185185185185E-3</c:v>
+                  <c:v>4.4444444444444398E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.0833333333333298E-3</c:v>
+                  <c:v>4.999999999999992E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.3148148148148099E-3</c:v>
+                  <c:v>5.5555555555555441E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.54629629629629E-3</c:v>
+                  <c:v>6.1111111111110963E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.7777777777777801E-3</c:v>
+                  <c:v>6.6666666666666721E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.0092592592592601E-3</c:v>
+                  <c:v>7.2222222222222243E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3.2407407407407402E-3</c:v>
+                  <c:v>7.7777777777777765E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.4722222222222199E-3</c:v>
+                  <c:v>8.3333333333333273E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.7037037037036999E-3</c:v>
+                  <c:v>8.8888888888888795E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.9351851851851796E-3</c:v>
+                  <c:v>9.4444444444444303E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4.1666666666666597E-3</c:v>
+                  <c:v>9.9999999999999839E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4.3981481481481502E-3</c:v>
+                  <c:v>0.1055555555555556</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4.6296296296296302E-3</c:v>
+                  <c:v>0.11111111111111113</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>4.8611111111111103E-3</c:v>
+                  <c:v>0.11666666666666664</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>5.0925925925925904E-3</c:v>
+                  <c:v>0.12222222222222218</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>5.3240740740740696E-3</c:v>
+                  <c:v>0.12777777777777766</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>5.5555555555555497E-3</c:v>
+                  <c:v>0.13333333333333319</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>5.7870370370370298E-3</c:v>
+                  <c:v>0.13888888888888873</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>6.0185185185185203E-3</c:v>
+                  <c:v>0.14444444444444449</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>6.2500000000000003E-3</c:v>
+                  <c:v>0.15000000000000002</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>6.4814814814814804E-3</c:v>
+                  <c:v>0.15555555555555553</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>6.7129629629629596E-3</c:v>
+                  <c:v>0.16111111111111104</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>6.9444444444444397E-3</c:v>
+                  <c:v>0.16666666666666655</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>7.1759259259259198E-3</c:v>
+                  <c:v>0.17222222222222208</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>7.4074074074074103E-3</c:v>
+                  <c:v>0.17777777777777784</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>7.6388888888888904E-3</c:v>
+                  <c:v>0.18333333333333338</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>7.8703703703703696E-3</c:v>
+                  <c:v>0.18888888888888888</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>8.1018518518518497E-3</c:v>
+                  <c:v>0.19444444444444439</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>8.3333333333333297E-3</c:v>
+                  <c:v>0.1999999999999999</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>8.5648148148148098E-3</c:v>
+                  <c:v>0.20555555555555544</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>8.7962962962962899E-3</c:v>
+                  <c:v>0.21111111111111097</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>9.0277777777777804E-3</c:v>
+                  <c:v>0.21666666666666673</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>9.2592592592592605E-3</c:v>
+                  <c:v>0.22222222222222227</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>9.4907407407407406E-3</c:v>
+                  <c:v>0.22777777777777777</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>9.7222222222222206E-3</c:v>
+                  <c:v>0.23333333333333328</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>9.9537037037037007E-3</c:v>
+                  <c:v>0.23888888888888882</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>1.01851851851852E-2</c:v>
+                  <c:v>0.2444444444444448</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>1.0416666666666701E-2</c:v>
+                  <c:v>0.25000000000000083</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>1.06481481481482E-2</c:v>
+                  <c:v>0.25555555555555681</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>1.08796296296296E-2</c:v>
+                  <c:v>0.26111111111111041</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>1.1111111111111099E-2</c:v>
+                  <c:v>0.26666666666666639</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>1.13425925925926E-2</c:v>
+                  <c:v>0.27222222222222242</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>1.1574074074074099E-2</c:v>
+                  <c:v>0.2777777777777784</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>1.18055555555556E-2</c:v>
+                  <c:v>0.28333333333333444</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>1.20370370370371E-2</c:v>
+                  <c:v>0.28888888888889042</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>1.22685185185185E-2</c:v>
+                  <c:v>0.29444444444444401</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>1.2500000000000001E-2</c:v>
+                  <c:v>0.30000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>1.27314814814815E-2</c:v>
+                  <c:v>0.30555555555555602</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>1.2962962962963001E-2</c:v>
+                  <c:v>0.311111111111112</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>1.31944444444445E-2</c:v>
+                  <c:v>0.31666666666666798</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>1.34259259259259E-2</c:v>
+                  <c:v>0.32222222222222163</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>1.3657407407407399E-2</c:v>
+                  <c:v>0.32777777777777761</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>1.38888888888889E-2</c:v>
+                  <c:v>0.33333333333333359</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>1.4120370370370399E-2</c:v>
+                  <c:v>0.33888888888888957</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>1.43518518518519E-2</c:v>
+                  <c:v>0.34444444444444561</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>1.4583333333333399E-2</c:v>
+                  <c:v>0.35000000000000159</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>1.48148148148148E-2</c:v>
+                  <c:v>0.35555555555555518</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>1.5046296296296301E-2</c:v>
+                  <c:v>0.36111111111111122</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>1.52777777777778E-2</c:v>
+                  <c:v>0.3666666666666672</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>1.5509259259259301E-2</c:v>
+                  <c:v>0.37222222222222323</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>1.5740740740740802E-2</c:v>
+                  <c:v>0.37777777777777921</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>1.59722222222222E-2</c:v>
+                  <c:v>0.3833333333333328</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>1.6203703703703699E-2</c:v>
+                  <c:v>0.38888888888888878</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>1.6435185185185198E-2</c:v>
+                  <c:v>0.39444444444444476</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>1.6666666666666701E-2</c:v>
+                  <c:v>0.4000000000000008</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>1.68981481481482E-2</c:v>
+                  <c:v>0.40555555555555678</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>1.7129629629629599E-2</c:v>
+                  <c:v>0.41111111111111037</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>1.7361111111111101E-2</c:v>
+                  <c:v>0.41666666666666641</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>1.7592592592592601E-2</c:v>
+                  <c:v>0.42222222222222239</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>1.78240740740741E-2</c:v>
+                  <c:v>0.42777777777777837</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>1.8055555555555599E-2</c:v>
+                  <c:v>0.43333333333333435</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>1.8287037037037102E-2</c:v>
+                  <c:v>0.43888888888889044</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>1.85185185185185E-2</c:v>
+                  <c:v>0.44444444444444398</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>1.8749999999999999E-2</c:v>
+                  <c:v>0.44999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>1.8981481481481498E-2</c:v>
+                  <c:v>0.45555555555555594</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>1.9212962962963001E-2</c:v>
+                  <c:v>0.46111111111111203</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>1.94444444444445E-2</c:v>
+                  <c:v>0.46666666666666801</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>1.9675925925925899E-2</c:v>
+                  <c:v>0.47222222222222154</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>1.9907407407407401E-2</c:v>
+                  <c:v>0.47777777777777763</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>2.0138888888888901E-2</c:v>
+                  <c:v>0.48333333333333361</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>2.03703703703704E-2</c:v>
+                  <c:v>0.48888888888888959</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>2.0601851851851899E-2</c:v>
+                  <c:v>0.49444444444444557</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>2.0833333333333402E-2</c:v>
+                  <c:v>0.50000000000000167</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>2.10648148148148E-2</c:v>
+                  <c:v>0.5055555555555552</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>2.1296296296296299E-2</c:v>
+                  <c:v>0.51111111111111118</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>2.1527777777777798E-2</c:v>
+                  <c:v>0.51666666666666716</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>2.1759259259259301E-2</c:v>
+                  <c:v>0.52222222222222325</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>2.19907407407408E-2</c:v>
+                  <c:v>0.52777777777777923</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>2.2222222222222199E-2</c:v>
+                  <c:v>0.53333333333333277</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>2.2453703703703701E-2</c:v>
+                  <c:v>0.53888888888888886</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>2.2685185185185201E-2</c:v>
+                  <c:v>0.54444444444444484</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>2.29166666666667E-2</c:v>
+                  <c:v>0.55000000000000082</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>2.3148148148148199E-2</c:v>
+                  <c:v>0.5555555555555568</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>2.3379629629629601E-2</c:v>
+                  <c:v>0.56111111111111045</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>2.36111111111111E-2</c:v>
+                  <c:v>0.56666666666666643</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>2.3842592592592599E-2</c:v>
+                  <c:v>0.57222222222222241</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>2.4074074074074098E-2</c:v>
+                  <c:v>0.57777777777777839</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>2.4305555555555601E-2</c:v>
+                  <c:v>0.58333333333333437</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>2.45370370370371E-2</c:v>
+                  <c:v>0.58888888888889035</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>2.4768518518518499E-2</c:v>
+                  <c:v>0.594444444444444</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>2.5000000000000001E-2</c:v>
+                  <c:v>0.60000000000000009</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>2.5231481481481501E-2</c:v>
+                  <c:v>0.60555555555555607</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>2.5462962962963E-2</c:v>
+                  <c:v>0.61111111111111205</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>2.5694444444444499E-2</c:v>
+                  <c:v>0.61666666666666803</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>2.5925925925925901E-2</c:v>
+                  <c:v>0.62222222222222157</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>2.61574074074074E-2</c:v>
+                  <c:v>0.62777777777777755</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>2.6388888888888899E-2</c:v>
+                  <c:v>0.63333333333333353</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>2.6620370370370398E-2</c:v>
+                  <c:v>0.63888888888888951</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>2.6851851851851901E-2</c:v>
+                  <c:v>0.6444444444444456</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>2.70833333333333E-2</c:v>
+                  <c:v>0.64999999999999925</c:v>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>2.7314814814814799E-2</c:v>
+                  <c:v>0.65555555555555522</c:v>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>2.7546296296296301E-2</c:v>
+                  <c:v>0.6611111111111112</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>2.7777777777777801E-2</c:v>
+                  <c:v>0.66666666666666718</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>2.80092592592593E-2</c:v>
+                  <c:v>0.67222222222222316</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>2.8240740740740799E-2</c:v>
+                  <c:v>0.67777777777777914</c:v>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>2.8472222222222201E-2</c:v>
+                  <c:v>0.68333333333333279</c:v>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>2.87037037037037E-2</c:v>
+                  <c:v>0.68888888888888877</c:v>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>2.8935185185185199E-2</c:v>
+                  <c:v>0.69444444444444475</c:v>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>2.9166666666666698E-2</c:v>
+                  <c:v>0.70000000000000073</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>2.9398148148148201E-2</c:v>
+                  <c:v>0.70555555555555682</c:v>
                 </c:pt>
                 <c:pt idx="127">
-                  <c:v>2.96296296296296E-2</c:v>
+                  <c:v>0.71111111111111036</c:v>
                 </c:pt>
                 <c:pt idx="128">
-                  <c:v>2.9861111111111099E-2</c:v>
+                  <c:v>0.71666666666666634</c:v>
                 </c:pt>
                 <c:pt idx="129">
-                  <c:v>3.0092592592592601E-2</c:v>
+                  <c:v>0.72222222222222243</c:v>
                 </c:pt>
                 <c:pt idx="130">
-                  <c:v>3.03240740740741E-2</c:v>
+                  <c:v>0.72777777777777841</c:v>
                 </c:pt>
                 <c:pt idx="131">
-                  <c:v>3.05555555555556E-2</c:v>
+                  <c:v>0.73333333333333439</c:v>
                 </c:pt>
                 <c:pt idx="132">
-                  <c:v>3.0787037037037099E-2</c:v>
+                  <c:v>0.73888888888889037</c:v>
                 </c:pt>
                 <c:pt idx="133">
-                  <c:v>3.1018518518518501E-2</c:v>
+                  <c:v>0.74444444444444402</c:v>
                 </c:pt>
                 <c:pt idx="134">
-                  <c:v>3.125E-2</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3188,7 +3117,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="0"/>
-          <c:order val="2"/>
+          <c:order val="1"/>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -3265,66 +3194,540 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>mass_conc!$A$43:$A$50</c:f>
+              <c:f>mass_conc!$D$50:$D$136</c:f>
               <c:numCache>
-                <c:formatCode>mm:ss</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="87"/>
                 <c:pt idx="0">
-                  <c:v>9.7222222222222206E-3</c:v>
+                  <c:v>0.27222222222222242</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.9537037037037007E-3</c:v>
+                  <c:v>0.2777777777777784</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.01851851851852E-2</c:v>
+                  <c:v>0.28333333333333444</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.0416666666666701E-2</c:v>
+                  <c:v>0.28888888888889042</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.06481481481482E-2</c:v>
+                  <c:v>0.29444444444444401</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.08796296296296E-2</c:v>
+                  <c:v>0.30000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.1111111111111099E-2</c:v>
+                  <c:v>0.30555555555555602</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.13425925925926E-2</c:v>
+                  <c:v>0.311111111111112</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.31666666666666798</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.32222222222222163</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.32777777777777761</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.33333333333333359</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.33888888888888957</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.34444444444444561</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.35000000000000159</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.35555555555555518</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.36111111111111122</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.3666666666666672</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.37222222222222323</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.37777777777777921</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.3833333333333328</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.38888888888888878</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.39444444444444476</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.4000000000000008</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.40555555555555678</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.41111111111111037</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.41666666666666641</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.42222222222222239</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.42777777777777837</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.43333333333333435</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.43888888888889044</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.44444444444444398</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.44999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.45555555555555594</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.46111111111111203</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.46666666666666801</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.47222222222222154</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.47777777777777763</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.48333333333333361</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.48888888888888959</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.49444444444444557</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.50000000000000167</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.5055555555555552</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.51111111111111118</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.51666666666666716</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.52222222222222325</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.52777777777777923</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.53333333333333277</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.53888888888888886</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.54444444444444484</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.55000000000000082</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.5555555555555568</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.56111111111111045</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.56666666666666643</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.57222222222222241</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.57777777777777839</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.58333333333333437</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.58888888888889035</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.594444444444444</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.60000000000000009</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.60555555555555607</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.61111111111111205</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.61666666666666803</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.62222222222222157</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.62777777777777755</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.63333333333333353</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.63888888888888951</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.6444444444444456</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.64999999999999925</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.65555555555555522</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.6611111111111112</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.66666666666666718</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.67222222222222316</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.67777777777777914</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.68333333333333279</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.68888888888888877</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.69444444444444475</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.70000000000000073</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.70555555555555682</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.71111111111111036</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.71666666666666634</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.72222222222222243</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.72777777777777841</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.73333333333333439</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.73888888888889037</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.74444444444444402</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>mass_conc!$B$43:$B$50</c:f>
+              <c:f>mass_conc!$B$50:$B$136</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="87"/>
                 <c:pt idx="0">
-                  <c:v>8.8846999999999995E-2</c:v>
+                  <c:v>2.0624300000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.61129E-2</c:v>
+                  <c:v>2.14284E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.6887399999999999E-2</c:v>
+                  <c:v>2.2241899999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.36373E-2</c:v>
+                  <c:v>2.1193300000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.2617999999999999E-2</c:v>
+                  <c:v>2.1445599999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.1260899999999999E-2</c:v>
+                  <c:v>1.97284E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.2346700000000001E-2</c:v>
+                  <c:v>1.9697599999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.0624300000000002E-2</c:v>
+                  <c:v>2.0802000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.9127999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.9599999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.0881799999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.77427E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.8108200000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.7759899999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.83083E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.8782199999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.8237E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.80144E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.7800199999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.7595599999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.7033699999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.6772700000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.7220599999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.63161E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.6228699999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1.7170500000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1.6586500000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.6978400000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.7223100000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.58581E-2</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.56119E-2</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>1.55566E-2</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1.5356699999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1.50169E-2</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1.50543E-2</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1.57961E-2</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1.50913E-2</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1.54427E-2</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1.51834E-2</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1.5082999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1.4970600000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1.51856E-2</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1.48387E-2</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1.4629700000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1.45215E-2</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1.5080700000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1.4664699999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1.49131E-2</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1.45685E-2</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1.4250799999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1.42311E-2</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1.41727E-2</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1.40424E-2</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1.3542800000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1.44171E-2</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1.42957E-2</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>1.39385E-2</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>1.40597E-2</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>1.34968E-2</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1.3901699999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>1.3880099999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>1.3290400000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1.2989000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1.3479E-2</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>1.2885499999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>1.3632E-2</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>1.2692500000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>1.2464599999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>1.28386E-2</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>1.30463E-2</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>1.27063E-2</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>1.3693500000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>1.24408E-2</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>1.2278300000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>1.49643E-2</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>1.20318E-2</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>1.22814E-2</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>1.2331399999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>1.14968E-2</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>1.2777699999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>1.18639E-2</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>1.24309E-2</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>1.21598E-2</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>1.2577E-2</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>1.17068E-2</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>1.14298E-2</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>1.16174E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3368,7 +3771,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="mm:ss" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -6662,16 +7065,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1536700</xdr:colOff>
-      <xdr:row>83</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>50800</xdr:colOff>
-      <xdr:row>115</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>114</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -40691,20 +41094,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C138"/>
+  <dimension ref="A1:D138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="P76" sqref="P76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
         <v>44</v>
       </c>
       <c r="B1" t="s">
@@ -40714,8 +41118,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="5">
         <v>2.3148148148148146E-4</v>
       </c>
       <c r="B2">
@@ -40724,9 +41128,13 @@
       <c r="C2">
         <v>3.6326900000000001E-3</v>
       </c>
+      <c r="D2" s="4">
+        <f>A2*24</f>
+        <v>5.5555555555555549E-3</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="5">
         <v>4.6296296296296293E-4</v>
       </c>
       <c r="B3">
@@ -40735,9 +41143,13 @@
       <c r="C3">
         <v>3.6382200000000002E-3</v>
       </c>
+      <c r="D3" s="4">
+        <f t="shared" ref="D3:D66" si="0">A3*24</f>
+        <v>1.111111111111111E-2</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="5">
         <v>6.9444444444444447E-4</v>
       </c>
       <c r="B4">
@@ -40746,9 +41158,13 @@
       <c r="C4">
         <v>3.3176199999999999E-3</v>
       </c>
+      <c r="D4" s="4">
+        <f t="shared" si="0"/>
+        <v>1.6666666666666666E-2</v>
+      </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="5">
         <v>9.2592592592592596E-4</v>
       </c>
       <c r="B5">
@@ -40757,9 +41173,13 @@
       <c r="C5">
         <v>4.7306400000000004E-3</v>
       </c>
+      <c r="D5" s="4">
+        <f t="shared" si="0"/>
+        <v>2.2222222222222223E-2</v>
+      </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="5">
         <v>1.1574074074074099E-3</v>
       </c>
       <c r="B6">
@@ -40768,9 +41188,13 @@
       <c r="C6">
         <v>3.1504699999999998E-3</v>
       </c>
+      <c r="D6" s="4">
+        <f t="shared" si="0"/>
+        <v>2.7777777777777839E-2</v>
+      </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="5">
         <v>1.38888888888889E-3</v>
       </c>
       <c r="B7">
@@ -40779,9 +41203,13 @@
       <c r="C7">
         <v>4.40472E-3</v>
       </c>
+      <c r="D7" s="4">
+        <f t="shared" si="0"/>
+        <v>3.3333333333333361E-2</v>
+      </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="5">
         <v>1.6203703703703701E-3</v>
       </c>
       <c r="B8">
@@ -40790,9 +41218,13 @@
       <c r="C8">
         <v>3.3522600000000001E-3</v>
       </c>
+      <c r="D8" s="4">
+        <f t="shared" si="0"/>
+        <v>3.8888888888888883E-2</v>
+      </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="5">
         <v>1.85185185185185E-3</v>
       </c>
       <c r="B9">
@@ -40801,9 +41233,13 @@
       <c r="C9">
         <v>5.31856E-3</v>
       </c>
+      <c r="D9" s="4">
+        <f t="shared" si="0"/>
+        <v>4.4444444444444398E-2</v>
+      </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="5">
         <v>2.0833333333333298E-3</v>
       </c>
       <c r="B10">
@@ -40812,9 +41248,13 @@
       <c r="C10">
         <v>4.1378300000000003E-3</v>
       </c>
+      <c r="D10" s="4">
+        <f t="shared" si="0"/>
+        <v>4.999999999999992E-2</v>
+      </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="5">
         <v>2.3148148148148099E-3</v>
       </c>
       <c r="B11">
@@ -40823,9 +41263,13 @@
       <c r="C11">
         <v>3.7037200000000002E-3</v>
       </c>
+      <c r="D11" s="4">
+        <f t="shared" si="0"/>
+        <v>5.5555555555555441E-2</v>
+      </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="5">
         <v>2.54629629629629E-3</v>
       </c>
       <c r="B12">
@@ -40834,9 +41278,13 @@
       <c r="C12">
         <v>3.9327199999999998E-3</v>
       </c>
+      <c r="D12" s="4">
+        <f t="shared" si="0"/>
+        <v>6.1111111111110963E-2</v>
+      </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="5">
         <v>2.7777777777777801E-3</v>
       </c>
       <c r="B13">
@@ -40845,9 +41293,13 @@
       <c r="C13">
         <v>3.2292599999999999E-3</v>
       </c>
+      <c r="D13" s="4">
+        <f t="shared" si="0"/>
+        <v>6.6666666666666721E-2</v>
+      </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="5">
         <v>3.0092592592592601E-3</v>
       </c>
       <c r="B14">
@@ -40856,9 +41308,13 @@
       <c r="C14">
         <v>4.6995700000000001E-3</v>
       </c>
+      <c r="D14" s="4">
+        <f t="shared" si="0"/>
+        <v>7.2222222222222243E-2</v>
+      </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="5">
         <v>3.2407407407407402E-3</v>
       </c>
       <c r="B15">
@@ -40867,9 +41323,13 @@
       <c r="C15">
         <v>3.2386200000000002E-3</v>
       </c>
+      <c r="D15" s="4">
+        <f t="shared" si="0"/>
+        <v>7.7777777777777765E-2</v>
+      </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="5">
         <v>3.4722222222222199E-3</v>
       </c>
       <c r="B16">
@@ -40878,9 +41338,13 @@
       <c r="C16">
         <v>3.2810199999999999E-3</v>
       </c>
+      <c r="D16" s="4">
+        <f t="shared" si="0"/>
+        <v>8.3333333333333273E-2</v>
+      </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="5">
         <v>3.7037037037036999E-3</v>
       </c>
       <c r="B17">
@@ -40889,9 +41353,13 @@
       <c r="C17">
         <v>4.0054499999999998E-3</v>
       </c>
+      <c r="D17" s="4">
+        <f t="shared" si="0"/>
+        <v>8.8888888888888795E-2</v>
+      </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="5">
         <v>3.9351851851851796E-3</v>
       </c>
       <c r="B18">
@@ -40900,9 +41368,13 @@
       <c r="C18">
         <v>6.7800100000000004E-3</v>
       </c>
+      <c r="D18" s="4">
+        <f t="shared" si="0"/>
+        <v>9.4444444444444303E-2</v>
+      </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="5">
         <v>4.1666666666666597E-3</v>
       </c>
       <c r="B19">
@@ -40911,9 +41383,13 @@
       <c r="C19">
         <v>1.8431300000000001E-2</v>
       </c>
+      <c r="D19" s="4">
+        <f t="shared" si="0"/>
+        <v>9.9999999999999839E-2</v>
+      </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="5">
         <v>4.3981481481481502E-3</v>
       </c>
       <c r="B20">
@@ -40922,9 +41398,13 @@
       <c r="C20">
         <v>2.7609399999999999E-2</v>
       </c>
+      <c r="D20" s="4">
+        <f t="shared" si="0"/>
+        <v>0.1055555555555556</v>
+      </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="5">
         <v>4.6296296296296302E-3</v>
       </c>
       <c r="B21">
@@ -40933,9 +41413,13 @@
       <c r="C21">
         <v>3.2138600000000003E-2</v>
       </c>
+      <c r="D21" s="4">
+        <f t="shared" si="0"/>
+        <v>0.11111111111111113</v>
+      </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="5">
         <v>4.8611111111111103E-3</v>
       </c>
       <c r="B22">
@@ -40944,9 +41428,13 @@
       <c r="C22">
         <v>4.2484899999999999E-2</v>
       </c>
+      <c r="D22" s="4">
+        <f t="shared" si="0"/>
+        <v>0.11666666666666664</v>
+      </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="5">
         <v>5.0925925925925904E-3</v>
       </c>
       <c r="B23">
@@ -40955,9 +41443,13 @@
       <c r="C23">
         <v>2.4558199999999999E-2</v>
       </c>
+      <c r="D23" s="4">
+        <f t="shared" si="0"/>
+        <v>0.12222222222222218</v>
+      </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="5">
         <v>5.3240740740740696E-3</v>
       </c>
       <c r="B24">
@@ -40966,9 +41458,13 @@
       <c r="C24">
         <v>1.4585000000000001E-2</v>
       </c>
+      <c r="D24" s="4">
+        <f t="shared" si="0"/>
+        <v>0.12777777777777766</v>
+      </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="5">
         <v>5.5555555555555497E-3</v>
       </c>
       <c r="B25">
@@ -40977,9 +41473,13 @@
       <c r="C25">
         <v>2.0382899999999999E-2</v>
       </c>
+      <c r="D25" s="4">
+        <f t="shared" si="0"/>
+        <v>0.13333333333333319</v>
+      </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="5">
         <v>5.7870370370370298E-3</v>
       </c>
       <c r="B26">
@@ -40988,9 +41488,13 @@
       <c r="C26">
         <v>4.0148900000000001E-2</v>
       </c>
+      <c r="D26" s="4">
+        <f t="shared" si="0"/>
+        <v>0.13888888888888873</v>
+      </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="5">
         <v>6.0185185185185203E-3</v>
       </c>
       <c r="B27">
@@ -40999,9 +41503,13 @@
       <c r="C27">
         <v>2.24432E-2</v>
       </c>
+      <c r="D27" s="4">
+        <f t="shared" si="0"/>
+        <v>0.14444444444444449</v>
+      </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="5">
         <v>6.2500000000000003E-3</v>
       </c>
       <c r="B28">
@@ -41010,9 +41518,13 @@
       <c r="C28">
         <v>3.0797399999999999E-2</v>
       </c>
+      <c r="D28" s="4">
+        <f t="shared" si="0"/>
+        <v>0.15000000000000002</v>
+      </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" s="5">
         <v>6.4814814814814804E-3</v>
       </c>
       <c r="B29">
@@ -41021,9 +41533,13 @@
       <c r="C29">
         <v>2.63187E-2</v>
       </c>
+      <c r="D29" s="4">
+        <f t="shared" si="0"/>
+        <v>0.15555555555555553</v>
+      </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" s="5">
         <v>6.7129629629629596E-3</v>
       </c>
       <c r="B30">
@@ -41032,9 +41548,13 @@
       <c r="C30">
         <v>3.67368E-2</v>
       </c>
+      <c r="D30" s="4">
+        <f t="shared" si="0"/>
+        <v>0.16111111111111104</v>
+      </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" s="5">
         <v>6.9444444444444397E-3</v>
       </c>
       <c r="B31">
@@ -41043,9 +41563,13 @@
       <c r="C31">
         <v>4.3904699999999998E-2</v>
       </c>
+      <c r="D31" s="4">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666655</v>
+      </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" s="5">
         <v>7.1759259259259198E-3</v>
       </c>
       <c r="B32">
@@ -41054,9 +41578,13 @@
       <c r="C32">
         <v>3.57373E-2</v>
       </c>
+      <c r="D32" s="4">
+        <f t="shared" si="0"/>
+        <v>0.17222222222222208</v>
+      </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="5">
         <v>7.4074074074074103E-3</v>
       </c>
       <c r="B33">
@@ -41065,9 +41593,13 @@
       <c r="C33">
         <v>4.1001599999999999E-2</v>
       </c>
+      <c r="D33" s="4">
+        <f t="shared" si="0"/>
+        <v>0.17777777777777784</v>
+      </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="5">
         <v>7.6388888888888904E-3</v>
       </c>
       <c r="B34">
@@ -41076,9 +41608,13 @@
       <c r="C34">
         <v>3.9562800000000002E-2</v>
       </c>
+      <c r="D34" s="4">
+        <f t="shared" si="0"/>
+        <v>0.18333333333333338</v>
+      </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="5">
         <v>7.8703703703703696E-3</v>
       </c>
       <c r="B35">
@@ -41087,9 +41623,13 @@
       <c r="C35">
         <v>4.0193399999999997E-2</v>
       </c>
+      <c r="D35" s="4">
+        <f t="shared" si="0"/>
+        <v>0.18888888888888888</v>
+      </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="5">
         <v>8.1018518518518497E-3</v>
       </c>
       <c r="B36">
@@ -41098,9 +41638,13 @@
       <c r="C36">
         <v>4.9366E-2</v>
       </c>
+      <c r="D36" s="4">
+        <f t="shared" si="0"/>
+        <v>0.19444444444444439</v>
+      </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" s="5">
         <v>8.3333333333333297E-3</v>
       </c>
       <c r="B37">
@@ -41109,9 +41653,13 @@
       <c r="C37">
         <v>4.7125899999999998E-2</v>
       </c>
+      <c r="D37" s="4">
+        <f t="shared" si="0"/>
+        <v>0.1999999999999999</v>
+      </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" s="5">
         <v>8.5648148148148098E-3</v>
       </c>
       <c r="B38">
@@ -41120,9 +41668,13 @@
       <c r="C38">
         <v>5.0790000000000002E-2</v>
       </c>
+      <c r="D38" s="4">
+        <f t="shared" si="0"/>
+        <v>0.20555555555555544</v>
+      </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" s="5">
         <v>8.7962962962962899E-3</v>
       </c>
       <c r="B39">
@@ -41131,9 +41683,13 @@
       <c r="C39">
         <v>4.99345E-2</v>
       </c>
+      <c r="D39" s="4">
+        <f t="shared" si="0"/>
+        <v>0.21111111111111097</v>
+      </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" s="5">
         <v>9.0277777777777804E-3</v>
       </c>
       <c r="B40">
@@ -41142,9 +41698,13 @@
       <c r="C40">
         <v>5.1772400000000003E-2</v>
       </c>
+      <c r="D40" s="4">
+        <f t="shared" si="0"/>
+        <v>0.21666666666666673</v>
+      </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" s="5">
         <v>9.2592592592592605E-3</v>
       </c>
       <c r="B41">
@@ -41153,9 +41713,13 @@
       <c r="C41">
         <v>4.3770799999999999E-2</v>
       </c>
+      <c r="D41" s="4">
+        <f t="shared" si="0"/>
+        <v>0.22222222222222227</v>
+      </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" s="5">
         <v>9.4907407407407406E-3</v>
       </c>
       <c r="B42">
@@ -41164,9 +41728,13 @@
       <c r="C42">
         <v>3.9608400000000002E-2</v>
       </c>
+      <c r="D42" s="4">
+        <f t="shared" si="0"/>
+        <v>0.22777777777777777</v>
+      </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" s="3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" s="5">
         <v>9.7222222222222206E-3</v>
       </c>
       <c r="B43">
@@ -41175,9 +41743,13 @@
       <c r="C43">
         <v>5.3033499999999997E-2</v>
       </c>
+      <c r="D43" s="4">
+        <f t="shared" si="0"/>
+        <v>0.23333333333333328</v>
+      </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" s="3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" s="5">
         <v>9.9537037037037007E-3</v>
       </c>
       <c r="B44">
@@ -41186,9 +41758,13 @@
       <c r="C44">
         <v>4.7620599999999999E-2</v>
       </c>
+      <c r="D44" s="4">
+        <f t="shared" si="0"/>
+        <v>0.23888888888888882</v>
+      </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" s="3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" s="5">
         <v>1.01851851851852E-2</v>
       </c>
       <c r="B45">
@@ -41197,9 +41773,13 @@
       <c r="C45">
         <v>3.1067399999999998E-2</v>
       </c>
+      <c r="D45" s="4">
+        <f t="shared" si="0"/>
+        <v>0.2444444444444448</v>
+      </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" s="5">
         <v>1.0416666666666701E-2</v>
       </c>
       <c r="B46">
@@ -41208,9 +41788,13 @@
       <c r="C46">
         <v>2.3914600000000001E-2</v>
       </c>
+      <c r="D46" s="4">
+        <f t="shared" si="0"/>
+        <v>0.25000000000000083</v>
+      </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="5">
         <v>1.06481481481482E-2</v>
       </c>
       <c r="B47">
@@ -41219,9 +41803,13 @@
       <c r="C47">
         <v>2.4178499999999999E-2</v>
       </c>
+      <c r="D47" s="4">
+        <f t="shared" si="0"/>
+        <v>0.25555555555555681</v>
+      </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" s="3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="5">
         <v>1.08796296296296E-2</v>
       </c>
       <c r="B48">
@@ -41230,9 +41818,13 @@
       <c r="C48">
         <v>2.4388799999999999E-2</v>
       </c>
+      <c r="D48" s="4">
+        <f t="shared" si="0"/>
+        <v>0.26111111111111041</v>
+      </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" s="3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="5">
         <v>1.1111111111111099E-2</v>
       </c>
       <c r="B49">
@@ -41241,9 +41833,13 @@
       <c r="C49">
         <v>2.42407E-2</v>
       </c>
+      <c r="D49" s="4">
+        <f t="shared" si="0"/>
+        <v>0.26666666666666639</v>
+      </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" s="3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="5">
         <v>1.13425925925926E-2</v>
       </c>
       <c r="B50">
@@ -41252,9 +41848,13 @@
       <c r="C50">
         <v>2.3558900000000001E-2</v>
       </c>
+      <c r="D50" s="4">
+        <f t="shared" si="0"/>
+        <v>0.27222222222222242</v>
+      </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" s="3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" s="5">
         <v>1.1574074074074099E-2</v>
       </c>
       <c r="B51">
@@ -41263,9 +41863,13 @@
       <c r="C51">
         <v>2.3538099999999999E-2</v>
       </c>
+      <c r="D51" s="4">
+        <f t="shared" si="0"/>
+        <v>0.2777777777777784</v>
+      </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" s="3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" s="5">
         <v>1.18055555555556E-2</v>
       </c>
       <c r="B52">
@@ -41274,9 +41878,13 @@
       <c r="C52">
         <v>2.5337200000000001E-2</v>
       </c>
+      <c r="D52" s="4">
+        <f t="shared" si="0"/>
+        <v>0.28333333333333444</v>
+      </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53" s="3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" s="5">
         <v>1.20370370370371E-2</v>
       </c>
       <c r="B53">
@@ -41285,9 +41893,13 @@
       <c r="C53">
         <v>2.5286300000000001E-2</v>
       </c>
+      <c r="D53" s="4">
+        <f t="shared" si="0"/>
+        <v>0.28888888888889042</v>
+      </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A54" s="3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" s="5">
         <v>1.22685185185185E-2</v>
       </c>
       <c r="B54">
@@ -41296,9 +41908,13 @@
       <c r="C54">
         <v>2.3800700000000001E-2</v>
       </c>
+      <c r="D54" s="4">
+        <f t="shared" si="0"/>
+        <v>0.29444444444444401</v>
+      </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55" s="3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" s="5">
         <v>1.2500000000000001E-2</v>
       </c>
       <c r="B55">
@@ -41307,9 +41923,13 @@
       <c r="C55">
         <v>2.30104E-2</v>
       </c>
+      <c r="D55" s="4">
+        <f t="shared" si="0"/>
+        <v>0.30000000000000004</v>
+      </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A56" s="3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" s="5">
         <v>1.27314814814815E-2</v>
       </c>
       <c r="B56">
@@ -41318,9 +41938,13 @@
       <c r="C56">
         <v>2.3153099999999999E-2</v>
       </c>
+      <c r="D56" s="4">
+        <f t="shared" si="0"/>
+        <v>0.30555555555555602</v>
+      </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57" s="3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" s="5">
         <v>1.2962962962963001E-2</v>
       </c>
       <c r="B57">
@@ -41329,9 +41953,13 @@
       <c r="C57">
         <v>2.2966899999999998E-2</v>
       </c>
+      <c r="D57" s="4">
+        <f t="shared" si="0"/>
+        <v>0.311111111111112</v>
+      </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A58" s="3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" s="5">
         <v>1.31944444444445E-2</v>
       </c>
       <c r="B58">
@@ -41340,9 +41968,13 @@
       <c r="C58">
         <v>2.1396499999999999E-2</v>
       </c>
+      <c r="D58" s="4">
+        <f t="shared" si="0"/>
+        <v>0.31666666666666798</v>
+      </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A59" s="3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59" s="5">
         <v>1.34259259259259E-2</v>
       </c>
       <c r="B59">
@@ -41351,9 +41983,13 @@
       <c r="C59">
         <v>2.15243E-2</v>
       </c>
+      <c r="D59" s="4">
+        <f t="shared" si="0"/>
+        <v>0.32222222222222163</v>
+      </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A60" s="3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" s="5">
         <v>1.3657407407407399E-2</v>
       </c>
       <c r="B60">
@@ -41362,9 +41998,13 @@
       <c r="C60">
         <v>2.0357299999999998E-2</v>
       </c>
+      <c r="D60" s="4">
+        <f t="shared" si="0"/>
+        <v>0.32777777777777761</v>
+      </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A61" s="3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" s="5">
         <v>1.38888888888889E-2</v>
       </c>
       <c r="B61">
@@ -41373,9 +42013,13 @@
       <c r="C61">
         <v>2.1589500000000001E-2</v>
       </c>
+      <c r="D61" s="4">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333359</v>
+      </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A62" s="3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" s="5">
         <v>1.4120370370370399E-2</v>
       </c>
       <c r="B62">
@@ -41384,9 +42028,13 @@
       <c r="C62">
         <v>2.0201799999999999E-2</v>
       </c>
+      <c r="D62" s="4">
+        <f t="shared" si="0"/>
+        <v>0.33888888888888957</v>
+      </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A63" s="3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" s="5">
         <v>1.43518518518519E-2</v>
       </c>
       <c r="B63">
@@ -41395,9 +42043,13 @@
       <c r="C63">
         <v>1.9680799999999998E-2</v>
       </c>
+      <c r="D63" s="4">
+        <f t="shared" si="0"/>
+        <v>0.34444444444444561</v>
+      </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A64" s="3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" s="5">
         <v>1.4583333333333399E-2</v>
       </c>
       <c r="B64">
@@ -41406,9 +42058,13 @@
       <c r="C64">
         <v>2.1660599999999999E-2</v>
       </c>
+      <c r="D64" s="4">
+        <f t="shared" si="0"/>
+        <v>0.35000000000000159</v>
+      </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A65" s="3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" s="5">
         <v>1.48148148148148E-2</v>
       </c>
       <c r="B65">
@@ -41417,9 +42073,13 @@
       <c r="C65">
         <v>2.0370900000000001E-2</v>
       </c>
+      <c r="D65" s="4">
+        <f t="shared" si="0"/>
+        <v>0.35555555555555518</v>
+      </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A66" s="3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A66" s="5">
         <v>1.5046296296296301E-2</v>
       </c>
       <c r="B66">
@@ -41428,9 +42088,13 @@
       <c r="C66">
         <v>1.9067299999999999E-2</v>
       </c>
+      <c r="D66" s="4">
+        <f t="shared" si="0"/>
+        <v>0.36111111111111122</v>
+      </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A67" s="3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A67" s="5">
         <v>1.52777777777778E-2</v>
       </c>
       <c r="B67">
@@ -41439,9 +42103,13 @@
       <c r="C67">
         <v>1.9205300000000002E-2</v>
       </c>
+      <c r="D67" s="4">
+        <f t="shared" ref="D67:D130" si="1">A67*24</f>
+        <v>0.3666666666666672</v>
+      </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A68" s="3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A68" s="5">
         <v>1.5509259259259301E-2</v>
       </c>
       <c r="B68">
@@ -41450,9 +42118,13 @@
       <c r="C68">
         <v>1.89252E-2</v>
       </c>
+      <c r="D68" s="4">
+        <f t="shared" si="1"/>
+        <v>0.37222222222222323</v>
+      </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A69" s="3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" s="5">
         <v>1.5740740740740802E-2</v>
       </c>
       <c r="B69">
@@ -41461,9 +42133,13 @@
       <c r="C69">
         <v>1.9504799999999999E-2</v>
       </c>
+      <c r="D69" s="4">
+        <f t="shared" si="1"/>
+        <v>0.37777777777777921</v>
+      </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A70" s="3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" s="5">
         <v>1.59722222222222E-2</v>
       </c>
       <c r="B70">
@@ -41472,9 +42148,13 @@
       <c r="C70">
         <v>1.9885E-2</v>
       </c>
+      <c r="D70" s="4">
+        <f t="shared" si="1"/>
+        <v>0.3833333333333328</v>
+      </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A71" s="3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" s="5">
         <v>1.6203703703703699E-2</v>
       </c>
       <c r="B71">
@@ -41483,9 +42163,13 @@
       <c r="C71">
         <v>1.8008400000000001E-2</v>
       </c>
+      <c r="D71" s="4">
+        <f t="shared" si="1"/>
+        <v>0.38888888888888878</v>
+      </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A72" s="3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" s="5">
         <v>1.6435185185185198E-2</v>
       </c>
       <c r="B72">
@@ -41494,9 +42178,13 @@
       <c r="C72">
         <v>1.8832000000000002E-2</v>
       </c>
+      <c r="D72" s="4">
+        <f t="shared" si="1"/>
+        <v>0.39444444444444476</v>
+      </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A73" s="3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" s="5">
         <v>1.6666666666666701E-2</v>
       </c>
       <c r="B73">
@@ -41505,9 +42193,13 @@
       <c r="C73">
         <v>1.79753E-2</v>
       </c>
+      <c r="D73" s="4">
+        <f t="shared" si="1"/>
+        <v>0.4000000000000008</v>
+      </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A74" s="3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74" s="5">
         <v>1.68981481481482E-2</v>
       </c>
       <c r="B74">
@@ -41516,9 +42208,13 @@
       <c r="C74">
         <v>1.8065999999999999E-2</v>
       </c>
+      <c r="D74" s="4">
+        <f t="shared" si="1"/>
+        <v>0.40555555555555678</v>
+      </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A75" s="3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" s="5">
         <v>1.7129629629629599E-2</v>
       </c>
       <c r="B75">
@@ -41527,9 +42223,13 @@
       <c r="C75">
         <v>1.8600200000000001E-2</v>
       </c>
+      <c r="D75" s="4">
+        <f t="shared" si="1"/>
+        <v>0.41111111111111037</v>
+      </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A76" s="3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76" s="5">
         <v>1.7361111111111101E-2</v>
       </c>
       <c r="B76">
@@ -41538,9 +42238,13 @@
       <c r="C76">
         <v>1.80406E-2</v>
       </c>
+      <c r="D76" s="4">
+        <f t="shared" si="1"/>
+        <v>0.41666666666666641</v>
+      </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A77" s="3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77" s="5">
         <v>1.7592592592592601E-2</v>
       </c>
       <c r="B77">
@@ -41549,9 +42253,13 @@
       <c r="C77">
         <v>1.7744699999999999E-2</v>
       </c>
+      <c r="D77" s="4">
+        <f t="shared" si="1"/>
+        <v>0.42222222222222239</v>
+      </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A78" s="3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78" s="5">
         <v>1.78240740740741E-2</v>
       </c>
       <c r="B78">
@@ -41560,9 +42268,13 @@
       <c r="C78">
         <v>1.82679E-2</v>
       </c>
+      <c r="D78" s="4">
+        <f t="shared" si="1"/>
+        <v>0.42777777777777837</v>
+      </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A79" s="3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A79" s="5">
         <v>1.8055555555555599E-2</v>
       </c>
       <c r="B79">
@@ -41571,9 +42283,13 @@
       <c r="C79">
         <v>1.8218999999999999E-2</v>
       </c>
+      <c r="D79" s="4">
+        <f t="shared" si="1"/>
+        <v>0.43333333333333435</v>
+      </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A80" s="3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80" s="5">
         <v>1.8287037037037102E-2</v>
       </c>
       <c r="B80">
@@ -41582,9 +42298,13 @@
       <c r="C80">
         <v>1.7785700000000002E-2</v>
       </c>
+      <c r="D80" s="4">
+        <f t="shared" si="1"/>
+        <v>0.43888888888889044</v>
+      </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A81" s="3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81" s="5">
         <v>1.85185185185185E-2</v>
       </c>
       <c r="B81">
@@ -41593,9 +42313,13 @@
       <c r="C81">
         <v>1.7359200000000002E-2</v>
       </c>
+      <c r="D81" s="4">
+        <f t="shared" si="1"/>
+        <v>0.44444444444444398</v>
+      </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A82" s="3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82" s="5">
         <v>1.8749999999999999E-2</v>
       </c>
       <c r="B82">
@@ -41604,9 +42328,13 @@
       <c r="C82">
         <v>1.7323000000000002E-2</v>
       </c>
+      <c r="D82" s="4">
+        <f t="shared" si="1"/>
+        <v>0.44999999999999996</v>
+      </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A83" s="3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83" s="5">
         <v>1.8981481481481498E-2</v>
       </c>
       <c r="B83">
@@ -41615,9 +42343,13 @@
       <c r="C83">
         <v>1.7062600000000001E-2</v>
       </c>
+      <c r="D83" s="4">
+        <f t="shared" si="1"/>
+        <v>0.45555555555555594</v>
+      </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A84" s="3">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A84" s="5">
         <v>1.9212962962963001E-2</v>
       </c>
       <c r="B84">
@@ -41626,9 +42358,13 @@
       <c r="C84">
         <v>1.7619900000000001E-2</v>
       </c>
+      <c r="D84" s="4">
+        <f t="shared" si="1"/>
+        <v>0.46111111111111203</v>
+      </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A85" s="3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A85" s="5">
         <v>1.94444444444445E-2</v>
       </c>
       <c r="B85">
@@ -41637,9 +42373,13 @@
       <c r="C85">
         <v>1.7243700000000001E-2</v>
       </c>
+      <c r="D85" s="4">
+        <f t="shared" si="1"/>
+        <v>0.46666666666666801</v>
+      </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A86" s="3">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A86" s="5">
         <v>1.9675925925925899E-2</v>
       </c>
       <c r="B86">
@@ -41648,9 +42388,13 @@
       <c r="C86">
         <v>1.6905400000000001E-2</v>
       </c>
+      <c r="D86" s="4">
+        <f t="shared" si="1"/>
+        <v>0.47222222222222154</v>
+      </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A87" s="3">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A87" s="5">
         <v>1.9907407407407401E-2</v>
       </c>
       <c r="B87">
@@ -41659,9 +42403,13 @@
       <c r="C87">
         <v>1.71358E-2</v>
       </c>
+      <c r="D87" s="4">
+        <f t="shared" si="1"/>
+        <v>0.47777777777777763</v>
+      </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A88" s="3">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A88" s="5">
         <v>2.0138888888888901E-2</v>
       </c>
       <c r="B88">
@@ -41670,9 +42418,13 @@
       <c r="C88">
         <v>1.8509500000000002E-2</v>
       </c>
+      <c r="D88" s="4">
+        <f t="shared" si="1"/>
+        <v>0.48333333333333361</v>
+      </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A89" s="3">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A89" s="5">
         <v>2.03703703703704E-2</v>
       </c>
       <c r="B89">
@@ -41681,9 +42433,13 @@
       <c r="C89">
         <v>2.06982E-2</v>
       </c>
+      <c r="D89" s="4">
+        <f t="shared" si="1"/>
+        <v>0.48888888888888959</v>
+      </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A90" s="3">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A90" s="5">
         <v>2.0601851851851899E-2</v>
       </c>
       <c r="B90">
@@ -41692,9 +42448,13 @@
       <c r="C90">
         <v>1.82043E-2</v>
       </c>
+      <c r="D90" s="4">
+        <f t="shared" si="1"/>
+        <v>0.49444444444444557</v>
+      </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A91" s="3">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A91" s="5">
         <v>2.0833333333333402E-2</v>
       </c>
       <c r="B91">
@@ -41703,9 +42463,13 @@
       <c r="C91">
         <v>1.80489E-2</v>
       </c>
+      <c r="D91" s="4">
+        <f t="shared" si="1"/>
+        <v>0.50000000000000167</v>
+      </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A92" s="3">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A92" s="5">
         <v>2.10648148148148E-2</v>
       </c>
       <c r="B92">
@@ -41714,9 +42478,13 @@
       <c r="C92">
         <v>1.7940999999999999E-2</v>
       </c>
+      <c r="D92" s="4">
+        <f t="shared" si="1"/>
+        <v>0.5055555555555552</v>
+      </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A93" s="3">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A93" s="5">
         <v>2.1296296296296299E-2</v>
       </c>
       <c r="B93">
@@ -41725,9 +42493,13 @@
       <c r="C93">
         <v>1.7803900000000001E-2</v>
       </c>
+      <c r="D93" s="4">
+        <f t="shared" si="1"/>
+        <v>0.51111111111111118</v>
+      </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A94" s="3">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A94" s="5">
         <v>2.1527777777777798E-2</v>
       </c>
       <c r="B94">
@@ -41736,9 +42508,13 @@
       <c r="C94">
         <v>1.9567899999999999E-2</v>
       </c>
+      <c r="D94" s="4">
+        <f t="shared" si="1"/>
+        <v>0.51666666666666716</v>
+      </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A95" s="3">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A95" s="5">
         <v>2.1759259259259301E-2</v>
       </c>
       <c r="B95">
@@ -41747,9 +42523,13 @@
       <c r="C95">
         <v>1.7153499999999999E-2</v>
       </c>
+      <c r="D95" s="4">
+        <f t="shared" si="1"/>
+        <v>0.52222222222222325</v>
+      </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A96" s="3">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A96" s="5">
         <v>2.19907407407408E-2</v>
       </c>
       <c r="B96">
@@ -41758,9 +42538,13 @@
       <c r="C96">
         <v>1.72584E-2</v>
       </c>
+      <c r="D96" s="4">
+        <f t="shared" si="1"/>
+        <v>0.52777777777777923</v>
+      </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A97" s="3">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A97" s="5">
         <v>2.2222222222222199E-2</v>
       </c>
       <c r="B97">
@@ -41769,9 +42553,13 @@
       <c r="C97">
         <v>1.6745900000000001E-2</v>
       </c>
+      <c r="D97" s="4">
+        <f t="shared" si="1"/>
+        <v>0.53333333333333277</v>
+      </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A98" s="3">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A98" s="5">
         <v>2.2453703703703701E-2</v>
       </c>
       <c r="B98">
@@ -41780,9 +42568,13 @@
       <c r="C98">
         <v>1.6183699999999999E-2</v>
       </c>
+      <c r="D98" s="4">
+        <f t="shared" si="1"/>
+        <v>0.53888888888888886</v>
+      </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A99" s="3">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A99" s="5">
         <v>2.2685185185185201E-2</v>
       </c>
       <c r="B99">
@@ -41791,9 +42583,13 @@
       <c r="C99">
         <v>1.6945499999999999E-2</v>
       </c>
+      <c r="D99" s="4">
+        <f t="shared" si="1"/>
+        <v>0.54444444444444484</v>
+      </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A100" s="3">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A100" s="5">
         <v>2.29166666666667E-2</v>
       </c>
       <c r="B100">
@@ -41802,9 +42598,13 @@
       <c r="C100">
         <v>1.6771299999999999E-2</v>
       </c>
+      <c r="D100" s="4">
+        <f t="shared" si="1"/>
+        <v>0.55000000000000082</v>
+      </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A101" s="3">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A101" s="5">
         <v>2.3148148148148199E-2</v>
       </c>
       <c r="B101">
@@ -41813,9 +42613,13 @@
       <c r="C101">
         <v>1.6958899999999999E-2</v>
       </c>
+      <c r="D101" s="4">
+        <f t="shared" si="1"/>
+        <v>0.5555555555555568</v>
+      </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A102" s="3">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A102" s="5">
         <v>2.3379629629629601E-2</v>
       </c>
       <c r="B102">
@@ -41824,9 +42628,13 @@
       <c r="C102">
         <v>1.6496799999999999E-2</v>
       </c>
+      <c r="D102" s="4">
+        <f t="shared" si="1"/>
+        <v>0.56111111111111045</v>
+      </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A103" s="3">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A103" s="5">
         <v>2.36111111111111E-2</v>
       </c>
       <c r="B103">
@@ -41835,9 +42643,13 @@
       <c r="C103">
         <v>1.6108399999999998E-2</v>
       </c>
+      <c r="D103" s="4">
+        <f t="shared" si="1"/>
+        <v>0.56666666666666643</v>
+      </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A104" s="3">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A104" s="5">
         <v>2.3842592592592599E-2</v>
       </c>
       <c r="B104">
@@ -41846,9 +42658,13 @@
       <c r="C104">
         <v>1.6557200000000001E-2</v>
       </c>
+      <c r="D104" s="4">
+        <f t="shared" si="1"/>
+        <v>0.57222222222222241</v>
+      </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A105" s="3">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A105" s="5">
         <v>2.4074074074074098E-2</v>
       </c>
       <c r="B105">
@@ -41857,9 +42673,13 @@
       <c r="C105">
         <v>1.6156500000000001E-2</v>
       </c>
+      <c r="D105" s="4">
+        <f t="shared" si="1"/>
+        <v>0.57777777777777839</v>
+      </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A106" s="3">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A106" s="5">
         <v>2.4305555555555601E-2</v>
       </c>
       <c r="B106">
@@ -41868,9 +42688,13 @@
       <c r="C106">
         <v>1.5723399999999998E-2</v>
       </c>
+      <c r="D106" s="4">
+        <f t="shared" si="1"/>
+        <v>0.58333333333333437</v>
+      </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A107" s="3">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A107" s="5">
         <v>2.45370370370371E-2</v>
       </c>
       <c r="B107">
@@ -41879,9 +42703,13 @@
       <c r="C107">
         <v>1.58119E-2</v>
       </c>
+      <c r="D107" s="4">
+        <f t="shared" si="1"/>
+        <v>0.58888888888889035</v>
+      </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A108" s="3">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A108" s="5">
         <v>2.4768518518518499E-2</v>
       </c>
       <c r="B108">
@@ -41890,9 +42718,13 @@
       <c r="C108">
         <v>1.5884300000000001E-2</v>
       </c>
+      <c r="D108" s="4">
+        <f t="shared" si="1"/>
+        <v>0.594444444444444</v>
+      </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A109" s="3">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A109" s="5">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="B109">
@@ -41901,9 +42733,13 @@
       <c r="C109">
         <v>1.5519399999999999E-2</v>
       </c>
+      <c r="D109" s="4">
+        <f t="shared" si="1"/>
+        <v>0.60000000000000009</v>
+      </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A110" s="3">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A110" s="5">
         <v>2.5231481481481501E-2</v>
       </c>
       <c r="B110">
@@ -41912,9 +42748,13 @@
       <c r="C110">
         <v>1.5995700000000002E-2</v>
       </c>
+      <c r="D110" s="4">
+        <f t="shared" si="1"/>
+        <v>0.60555555555555607</v>
+      </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A111" s="3">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A111" s="5">
         <v>2.5462962962963E-2</v>
       </c>
       <c r="B111">
@@ -41923,9 +42763,13 @@
       <c r="C111">
         <v>1.5526099999999999E-2</v>
       </c>
+      <c r="D111" s="4">
+        <f t="shared" si="1"/>
+        <v>0.61111111111111205</v>
+      </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A112" s="3">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A112" s="5">
         <v>2.5694444444444499E-2</v>
       </c>
       <c r="B112">
@@ -41934,9 +42778,13 @@
       <c r="C112">
         <v>1.54763E-2</v>
       </c>
+      <c r="D112" s="4">
+        <f t="shared" si="1"/>
+        <v>0.61666666666666803</v>
+      </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A113" s="3">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A113" s="5">
         <v>2.5925925925925901E-2</v>
       </c>
       <c r="B113">
@@ -41945,9 +42793,13 @@
       <c r="C113">
         <v>1.5898800000000001E-2</v>
       </c>
+      <c r="D113" s="4">
+        <f t="shared" si="1"/>
+        <v>0.62222222222222157</v>
+      </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A114" s="3">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A114" s="5">
         <v>2.61574074074074E-2</v>
       </c>
       <c r="B114">
@@ -41956,9 +42808,13 @@
       <c r="C114">
         <v>1.5093199999999999E-2</v>
       </c>
+      <c r="D114" s="4">
+        <f t="shared" si="1"/>
+        <v>0.62777777777777755</v>
+      </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A115" s="3">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A115" s="5">
         <v>2.6388888888888899E-2</v>
       </c>
       <c r="B115">
@@ -41967,9 +42823,13 @@
       <c r="C115">
         <v>1.4452100000000001E-2</v>
       </c>
+      <c r="D115" s="4">
+        <f t="shared" si="1"/>
+        <v>0.63333333333333353</v>
+      </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A116" s="3">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A116" s="5">
         <v>2.6620370370370398E-2</v>
       </c>
       <c r="B116">
@@ -41978,9 +42838,13 @@
       <c r="C116">
         <v>1.4755300000000001E-2</v>
       </c>
+      <c r="D116" s="4">
+        <f t="shared" si="1"/>
+        <v>0.63888888888888951</v>
+      </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A117" s="3">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A117" s="5">
         <v>2.6851851851851901E-2</v>
       </c>
       <c r="B117">
@@ -41989,9 +42853,13 @@
       <c r="C117">
         <v>1.4801099999999999E-2</v>
       </c>
+      <c r="D117" s="4">
+        <f t="shared" si="1"/>
+        <v>0.6444444444444456</v>
+      </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A118" s="3">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A118" s="5">
         <v>2.70833333333333E-2</v>
       </c>
       <c r="B118">
@@ -42000,9 +42868,13 @@
       <c r="C118">
         <v>1.4327100000000001E-2</v>
       </c>
+      <c r="D118" s="4">
+        <f t="shared" si="1"/>
+        <v>0.64999999999999925</v>
+      </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A119" s="3">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A119" s="5">
         <v>2.7314814814814799E-2</v>
       </c>
       <c r="B119">
@@ -42011,9 +42883,13 @@
       <c r="C119">
         <v>1.5821999999999999E-2</v>
       </c>
+      <c r="D119" s="4">
+        <f t="shared" si="1"/>
+        <v>0.65555555555555522</v>
+      </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A120" s="3">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A120" s="5">
         <v>2.7546296296296301E-2</v>
       </c>
       <c r="B120">
@@ -42022,9 +42898,13 @@
       <c r="C120">
         <v>1.46035E-2</v>
       </c>
+      <c r="D120" s="4">
+        <f t="shared" si="1"/>
+        <v>0.6611111111111112</v>
+      </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A121" s="3">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A121" s="5">
         <v>2.7777777777777801E-2</v>
       </c>
       <c r="B121">
@@ -42033,9 +42913,13 @@
       <c r="C121">
         <v>1.44993E-2</v>
       </c>
+      <c r="D121" s="4">
+        <f t="shared" si="1"/>
+        <v>0.66666666666666718</v>
+      </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A122" s="3">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A122" s="5">
         <v>2.80092592592593E-2</v>
       </c>
       <c r="B122">
@@ -42044,9 +42928,13 @@
       <c r="C122">
         <v>1.48247E-2</v>
       </c>
+      <c r="D122" s="4">
+        <f t="shared" si="1"/>
+        <v>0.67222222222222316</v>
+      </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A123" s="3">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A123" s="5">
         <v>2.8240740740740799E-2</v>
       </c>
       <c r="B123">
@@ -42055,9 +42943,13 @@
       <c r="C123">
         <v>1.4504299999999999E-2</v>
       </c>
+      <c r="D123" s="4">
+        <f t="shared" si="1"/>
+        <v>0.67777777777777914</v>
+      </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A124" s="3">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A124" s="5">
         <v>2.8472222222222201E-2</v>
       </c>
       <c r="B124">
@@ -42066,9 +42958,13 @@
       <c r="C124">
         <v>1.4482E-2</v>
       </c>
+      <c r="D124" s="4">
+        <f t="shared" si="1"/>
+        <v>0.68333333333333279</v>
+      </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A125" s="3">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A125" s="5">
         <v>2.87037037037037E-2</v>
       </c>
       <c r="B125">
@@ -42077,9 +42973,13 @@
       <c r="C125">
         <v>1.4146300000000001E-2</v>
       </c>
+      <c r="D125" s="4">
+        <f t="shared" si="1"/>
+        <v>0.68888888888888877</v>
+      </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A126" s="3">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A126" s="5">
         <v>2.8935185185185199E-2</v>
       </c>
       <c r="B126">
@@ -42088,9 +42988,13 @@
       <c r="C126">
         <v>1.4037600000000001E-2</v>
       </c>
+      <c r="D126" s="4">
+        <f t="shared" si="1"/>
+        <v>0.69444444444444475</v>
+      </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A127" s="3">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A127" s="5">
         <v>2.9166666666666698E-2</v>
       </c>
       <c r="B127">
@@ -42099,9 +43003,13 @@
       <c r="C127">
         <v>1.3447799999999999E-2</v>
       </c>
+      <c r="D127" s="4">
+        <f t="shared" si="1"/>
+        <v>0.70000000000000073</v>
+      </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A128" s="3">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A128" s="5">
         <v>2.9398148148148201E-2</v>
       </c>
       <c r="B128">
@@ -42110,9 +43018,13 @@
       <c r="C128">
         <v>1.4321E-2</v>
       </c>
+      <c r="D128" s="4">
+        <f t="shared" si="1"/>
+        <v>0.70555555555555682</v>
+      </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A129" s="3">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A129" s="5">
         <v>2.96296296296296E-2</v>
       </c>
       <c r="B129">
@@ -42121,9 +43033,13 @@
       <c r="C129">
         <v>1.3457200000000001E-2</v>
       </c>
+      <c r="D129" s="4">
+        <f t="shared" si="1"/>
+        <v>0.71111111111111036</v>
+      </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A130" s="3">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A130" s="5">
         <v>2.9861111111111099E-2</v>
       </c>
       <c r="B130">
@@ -42132,9 +43048,13 @@
       <c r="C130">
         <v>1.39189E-2</v>
       </c>
+      <c r="D130" s="4">
+        <f t="shared" si="1"/>
+        <v>0.71666666666666634</v>
+      </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A131" s="3">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A131" s="5">
         <v>3.0092592592592601E-2</v>
       </c>
       <c r="B131">
@@ -42143,9 +43063,13 @@
       <c r="C131">
         <v>1.4188600000000001E-2</v>
       </c>
+      <c r="D131" s="4">
+        <f t="shared" ref="D131:D136" si="2">A131*24</f>
+        <v>0.72222222222222243</v>
+      </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A132" s="3">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A132" s="5">
         <v>3.03240740740741E-2</v>
       </c>
       <c r="B132">
@@ -42154,9 +43078,13 @@
       <c r="C132">
         <v>1.4002300000000001E-2</v>
       </c>
+      <c r="D132" s="4">
+        <f t="shared" si="2"/>
+        <v>0.72777777777777841</v>
+      </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A133" s="3">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A133" s="5">
         <v>3.05555555555556E-2</v>
       </c>
       <c r="B133">
@@ -42165,9 +43093,13 @@
       <c r="C133">
         <v>1.3887099999999999E-2</v>
       </c>
+      <c r="D133" s="4">
+        <f t="shared" si="2"/>
+        <v>0.73333333333333439</v>
+      </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A134" s="3">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A134" s="5">
         <v>3.0787037037037099E-2</v>
       </c>
       <c r="B134">
@@ -42176,9 +43108,13 @@
       <c r="C134">
         <v>1.42621E-2</v>
       </c>
+      <c r="D134" s="4">
+        <f t="shared" si="2"/>
+        <v>0.73888888888889037</v>
+      </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A135" s="3">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A135" s="5">
         <v>3.1018518518518501E-2</v>
       </c>
       <c r="B135">
@@ -42187,9 +43123,13 @@
       <c r="C135">
         <v>1.3329000000000001E-2</v>
       </c>
+      <c r="D135" s="4">
+        <f t="shared" si="2"/>
+        <v>0.74444444444444402</v>
+      </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A136" s="3">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A136" s="5">
         <v>3.125E-2</v>
       </c>
       <c r="B136">
@@ -42198,9 +43138,13 @@
       <c r="C136">
         <v>1.35476E-2</v>
       </c>
+      <c r="D136" s="4">
+        <f t="shared" si="2"/>
+        <v>0.75</v>
+      </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A138" t="s">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A138" s="5" t="s">
         <v>45</v>
       </c>
       <c r="B138">
@@ -43749,12 +44693,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -43763,7 +44701,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010063F3C2B24EE74845B032A2CC0F813651" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="926914e20f5f300737307ea7be0184e1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="dcdbe96c-9c47-4202-80f5-cac5e6e6d6c1" xmlns:ns4="1e8eff21-aac5-419e-8496-4266dd95c283" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2d2603b88a961a7e06a76e94fde58845" ns3:_="" ns4:_="">
     <xsd:import namespace="dcdbe96c-9c47-4202-80f5-cac5e6e6d6c1"/>
@@ -43980,24 +44918,13 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4FA8A0D-417C-4577-9A5A-39B711A4238C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="dcdbe96c-9c47-4202-80f5-cac5e6e6d6c1"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="1e8eff21-aac5-419e-8496-4266dd95c283"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DC804984-24DD-47D8-B978-D9B6EA987778}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -44005,7 +44932,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E9559CC0-1BA7-4F4A-B0F5-5D8CA041055D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -44022,4 +44949,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4FA8A0D-417C-4577-9A5A-39B711A4238C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="dcdbe96c-9c47-4202-80f5-cac5e6e6d6c1"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="1e8eff21-aac5-419e-8496-4266dd95c283"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>